<commit_message>
[ADD] phylogenetic_tree curation [WILDCARD] A thermonuclear detonation.
</commit_message>
<xml_diff>
--- a/organisms_rna/organisms_to_curate.xlsx
+++ b/organisms_rna/organisms_to_curate.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/Papers/bit analysis/bit-analysis/organisms_rna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="11_F25DC773A252ABDACC10485AD91858DA5ADE58EE" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BC1BD95D-1D24-44BD-8F8D-5CAC1C676F52}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_F25DC773A252ABDACC10485AD91858DA5ADE58EE" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{956FA1F4-3D62-4CF8-84D2-2C31077AAA22}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$24</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="69">
   <si>
     <t>Bigg ID</t>
   </si>
@@ -210,7 +213,28 @@
     <t xml:space="preserve"> GCF_015475595.1</t>
   </si>
   <si>
-    <t xml:space="preserve"> ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/015/475/595/GCA_015475595.1_ASM1547559v1</t>
+    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/002/415/GCA_000002415.2_ASM241v2/</t>
+  </si>
+  <si>
+    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/011/392/055/GCA_011392055.1_ASM1139205v1/</t>
+  </si>
+  <si>
+    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/001/293/415/GCA_001293415.1_ASM129341v1/</t>
+  </si>
+  <si>
+    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/012/005/GCA_000012005.1_ASM1200v1/</t>
+  </si>
+  <si>
+    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/002/595/GCA_000002595.2_v3.0/</t>
+  </si>
+  <si>
+    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/013/167/015/GCA_013167015.1_ASM1316701v1/</t>
+  </si>
+  <si>
+    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/023/665/GCA_000023665.1_ASM2366v1/</t>
+  </si>
+  <si>
+    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/008/865/GCA_000008865.2_ASM886v2/</t>
   </si>
 </sst>
 </file>
@@ -531,7 +555,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,7 +619,7 @@
         <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -621,15 +645,15 @@
         <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>53</v>
@@ -647,12 +671,12 @@
         <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -673,15 +697,15 @@
         <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
         <v>53</v>
@@ -699,15 +723,15 @@
         <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>53</v>
@@ -730,10 +754,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>53</v>
@@ -756,10 +780,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>53</v>
@@ -782,10 +806,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>53</v>
@@ -808,10 +832,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
         <v>53</v>
@@ -834,10 +858,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
         <v>53</v>
@@ -860,10 +884,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
         <v>53</v>
@@ -907,7 +931,7 @@
         <v>31</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -938,10 +962,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
         <v>53</v>
@@ -985,15 +1009,15 @@
         <v>31</v>
       </c>
       <c r="H17" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
         <v>53</v>
@@ -1037,7 +1061,7 @@
         <v>31</v>
       </c>
       <c r="H19" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1063,7 +1087,7 @@
         <v>31</v>
       </c>
       <c r="H20" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1089,7 +1113,7 @@
         <v>32</v>
       </c>
       <c r="H21" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1115,15 +1139,15 @@
         <v>31</v>
       </c>
       <c r="H22" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
         <v>53</v>
@@ -1146,10 +1170,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
         <v>53</v>
@@ -1171,6 +1195,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H24" xr:uid="{49BA6B57-A8C6-4E37-8E78-5DAADA36DA8F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H24">
+      <sortCondition ref="B1:B24"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>